<commit_message>
Added debug level functionality for milestone 2
</commit_message>
<xml_diff>
--- a/development_schedule.xlsx
+++ b/development_schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="46">
   <si>
     <t>Task</t>
   </si>
@@ -315,6 +315,44 @@
   </si>
   <si>
     <t>Building an automated workload capable of running realistic transaction on a database, on a schedule.</t>
+  </si>
+  <si>
+    <t>Milestone 2 Testing &amp; Evaluation</t>
+  </si>
+  <si>
+    <r>
+      <t>Evaluation for milestone 2 components (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Peak Load, Stats Priority, Optimizer Stats Generation Time Estimate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> models)</t>
+    </r>
+  </si>
+  <si>
+    <t>Milestone 3</t>
+  </si>
+  <si>
+    <t>Write-Up</t>
+  </si>
+  <si>
+    <t>Compile Write Up</t>
   </si>
 </sst>
 </file>
@@ -708,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,37 +1262,54 @@
         <v>4</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="7" t="s">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
+        <v>29</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="3" t="s">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="4" t="s">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>